<commit_message>
Add form detail page
</commit_message>
<xml_diff>
--- a/app-designer/app/config/tables/cha/forms/cha/cha.xlsx
+++ b/app-designer/app/config/tables/cha/forms/cha/cha.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="169">
   <si>
     <t xml:space="preserve">setting_name</t>
   </si>
@@ -521,6 +521,15 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detailViewFileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config/tables/cha/html/cha_detail.html</t>
   </si>
 </sst>
 </file>
@@ -531,7 +540,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -566,11 +575,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -615,7 +619,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -634,10 +638,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -734,7 +734,7 @@
   </sheetPr>
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F67" activeCellId="0" sqref="F67"/>
     </sheetView>
   </sheetViews>
@@ -746,7 +746,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1252,7 +1252,7 @@
       <c r="B39" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="5"/>
+      <c r="H39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
@@ -1261,7 +1261,7 @@
       <c r="C40" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H40" s="5"/>
+      <c r="H40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
@@ -1271,7 +1271,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="5"/>
+      <c r="H41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="0" t="s">
@@ -1776,7 +1776,7 @@
       <c r="B14" s="0" t="n">
         <v>2019</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       <c r="B15" s="0" t="n">
         <v>2020</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1798,7 +1798,7 @@
       <c r="B16" s="0" t="n">
         <v>2021</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1862,10 +1862,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1909,6 +1909,23 @@
         <v>165</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Put date on its own page
</commit_message>
<xml_diff>
--- a/app-designer/app/config/tables/cha/forms/cha/cha.xlsx
+++ b/app-designer/app/config/tables/cha/forms/cha/cha.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="169">
   <si>
     <t xml:space="preserve">setting_name</t>
   </si>
@@ -97,6 +97,9 @@
     <t xml:space="preserve">Today’s Date:</t>
   </si>
   <si>
+    <t xml:space="preserve">end screen</t>
+  </si>
+  <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
@@ -122,9 +125,6 @@
   </si>
   <si>
     <t xml:space="preserve">Your (CHA) Name:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end screen</t>
   </si>
   <si>
     <t xml:space="preserve">select_one</t>
@@ -646,12 +646,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -732,10 +732,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F67" activeCellId="0" sqref="F67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -811,44 +811,24 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="B6" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -857,13 +837,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -871,52 +851,43 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="0" t="n">
+      <c r="D9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I11" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="0" t="n">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>41</v>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,62 +895,73 @@
         <v>34</v>
       </c>
       <c r="E13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I15" s="0" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -987,10 +969,10 @@
         <v>47</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>50</v>
@@ -1001,10 +983,10 @@
         <v>47</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>50</v>
@@ -1015,10 +997,10 @@
         <v>47</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>50</v>
@@ -1029,10 +1011,10 @@
         <v>47</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>50</v>
@@ -1043,10 +1025,10 @@
         <v>47</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>50</v>
@@ -1057,10 +1039,10 @@
         <v>47</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>50</v>
@@ -1071,10 +1053,10 @@
         <v>47</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>50</v>
@@ -1085,10 +1067,10 @@
         <v>47</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>50</v>
@@ -1099,74 +1081,74 @@
         <v>47</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>33</v>
+      <c r="D28" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>71</v>
+      <c r="D29" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>74</v>
@@ -1177,10 +1159,10 @@
         <v>47</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>74</v>
@@ -1191,10 +1173,10 @@
         <v>47</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>74</v>
@@ -1205,13 +1187,10 @@
         <v>47</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>74</v>
@@ -1222,13 +1201,10 @@
         <v>47</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>74</v>
@@ -1239,77 +1215,83 @@
         <v>47</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="H39" s="2"/>
+      <c r="D39" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H40" s="2"/>
+      <c r="D40" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="2"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>94</v>
@@ -1320,10 +1302,10 @@
         <v>47</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>94</v>
@@ -1334,10 +1316,10 @@
         <v>47</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>94</v>
@@ -1348,10 +1330,10 @@
         <v>47</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>94</v>
@@ -1362,10 +1344,10 @@
         <v>47</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>94</v>
@@ -1376,10 +1358,10 @@
         <v>47</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>94</v>
@@ -1390,10 +1372,10 @@
         <v>47</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>94</v>
@@ -1404,10 +1386,10 @@
         <v>47</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>94</v>
@@ -1418,10 +1400,10 @@
         <v>47</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>94</v>
@@ -1432,10 +1414,10 @@
         <v>47</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>94</v>
@@ -1446,10 +1428,10 @@
         <v>47</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>94</v>
@@ -1460,74 +1442,74 @@
         <v>47</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
-        <v>33</v>
+      <c r="D56" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>121</v>
+      <c r="D57" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F59" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D61" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>124</v>
@@ -1538,10 +1520,10 @@
         <v>47</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>124</v>
@@ -1552,10 +1534,10 @@
         <v>47</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>124</v>
@@ -1566,33 +1548,61 @@
         <v>47</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
-        <v>33</v>
+      <c r="D65" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="H65" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="D66" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="0" t="s">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D69" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F67" s="0" t="s">
+      <c r="F69" s="0" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1864,7 +1874,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>